<commit_message>
Added unit test for WorkersMessagesTest.py and NotesTkinter
</commit_message>
<xml_diff>
--- a/TestDatabase.xlsx
+++ b/TestDatabase.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="10" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8055" windowWidth="21570" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="14" autoFilterDateGrouping="1" firstSheet="3" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8055" windowWidth="21570" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Cities Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,6 +18,11 @@
     <sheet name="Dimona" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Giv'at Ze'ev" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Arad" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Test" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="asfgfasf" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Test22" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Test23" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -26,14 +31,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt formatCode="m/d/yyyy;@" numFmtId="164"/>
     <numFmt formatCode="0;[Red]0" numFmtId="165"/>
-    <numFmt formatCode="dd\-mm\-yyyy" numFmtId="166"/>
+    <numFmt formatCode="[$-14C09]dd/mm/yyyy;@" numFmtId="166"/>
     <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="167"/>
-    <numFmt formatCode="[$-14C09]dd/mm/yyyy;@" numFmtId="168"/>
+    <numFmt formatCode="dd\-mm\-yyyy" numFmtId="168"/>
     <numFmt formatCode="yyyy/mm/dd;@" numFmtId="169"/>
     <numFmt formatCode="DD-MM-YYYY" numFmtId="170"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="171"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -323,17 +329,17 @@
     <xf borderId="1" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="8" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="169" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="169" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="170" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="171" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2389,10 +2395,10 @@
       <c r="D2" s="25" t="n">
         <v>123456789</v>
       </c>
-      <c r="E2" s="36" t="n">
+      <c r="E2" s="37" t="n">
         <v>21099</v>
       </c>
-      <c r="F2" s="36" t="n">
+      <c r="F2" s="37" t="n">
         <v>44158</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -2413,128 +2419,128 @@
     </row>
     <row r="3">
       <c r="D3" s="25" t="n"/>
-      <c r="E3" s="36" t="n"/>
-      <c r="F3" s="36" t="n"/>
+      <c r="E3" s="37" t="n"/>
+      <c r="F3" s="37" t="n"/>
     </row>
     <row r="4">
       <c r="D4" s="25" t="n"/>
-      <c r="E4" s="36" t="n"/>
-      <c r="F4" s="36" t="n"/>
+      <c r="E4" s="37" t="n"/>
+      <c r="F4" s="37" t="n"/>
     </row>
     <row r="5">
       <c r="D5" s="25" t="n"/>
-      <c r="E5" s="36" t="n"/>
-      <c r="F5" s="36" t="n"/>
+      <c r="E5" s="37" t="n"/>
+      <c r="F5" s="37" t="n"/>
     </row>
     <row r="6">
       <c r="D6" s="25" t="n"/>
-      <c r="E6" s="36" t="n"/>
-      <c r="F6" s="36" t="n"/>
+      <c r="E6" s="37" t="n"/>
+      <c r="F6" s="37" t="n"/>
     </row>
     <row r="7">
       <c r="D7" s="25" t="n"/>
-      <c r="E7" s="36" t="n"/>
-      <c r="F7" s="36" t="n"/>
+      <c r="E7" s="37" t="n"/>
+      <c r="F7" s="37" t="n"/>
     </row>
     <row r="8">
       <c r="D8" s="25" t="n"/>
-      <c r="E8" s="36" t="n"/>
-      <c r="F8" s="36" t="n"/>
+      <c r="E8" s="37" t="n"/>
+      <c r="F8" s="37" t="n"/>
     </row>
     <row r="9">
       <c r="D9" s="25" t="n"/>
-      <c r="E9" s="36" t="n"/>
-      <c r="F9" s="36" t="n"/>
+      <c r="E9" s="37" t="n"/>
+      <c r="F9" s="37" t="n"/>
     </row>
     <row r="10">
       <c r="D10" s="25" t="n"/>
-      <c r="E10" s="36" t="n"/>
-      <c r="F10" s="36" t="n"/>
+      <c r="E10" s="37" t="n"/>
+      <c r="F10" s="37" t="n"/>
     </row>
     <row r="11">
       <c r="D11" s="25" t="n"/>
-      <c r="E11" s="36" t="n"/>
-      <c r="F11" s="36" t="n"/>
+      <c r="E11" s="37" t="n"/>
+      <c r="F11" s="37" t="n"/>
     </row>
     <row r="12">
       <c r="D12" s="25" t="n"/>
-      <c r="E12" s="36" t="n"/>
-      <c r="F12" s="36" t="n"/>
+      <c r="E12" s="37" t="n"/>
+      <c r="F12" s="37" t="n"/>
     </row>
     <row r="13">
       <c r="D13" s="25" t="n"/>
-      <c r="E13" s="36" t="n"/>
-      <c r="F13" s="36" t="n"/>
+      <c r="E13" s="37" t="n"/>
+      <c r="F13" s="37" t="n"/>
     </row>
     <row r="14">
       <c r="D14" s="25" t="n"/>
-      <c r="E14" s="36" t="n"/>
-      <c r="F14" s="36" t="n"/>
+      <c r="E14" s="37" t="n"/>
+      <c r="F14" s="37" t="n"/>
     </row>
     <row r="15">
       <c r="D15" s="25" t="n"/>
-      <c r="E15" s="36" t="n"/>
-      <c r="F15" s="36" t="n"/>
+      <c r="E15" s="37" t="n"/>
+      <c r="F15" s="37" t="n"/>
     </row>
     <row r="16">
       <c r="D16" s="25" t="n"/>
-      <c r="E16" s="36" t="n"/>
-      <c r="F16" s="36" t="n"/>
+      <c r="E16" s="37" t="n"/>
+      <c r="F16" s="37" t="n"/>
     </row>
     <row r="17">
       <c r="D17" s="25" t="n"/>
-      <c r="E17" s="36" t="n"/>
-      <c r="F17" s="36" t="n"/>
+      <c r="E17" s="37" t="n"/>
+      <c r="F17" s="37" t="n"/>
     </row>
     <row r="18">
       <c r="D18" s="25" t="n"/>
-      <c r="E18" s="36" t="n"/>
-      <c r="F18" s="36" t="n"/>
+      <c r="E18" s="37" t="n"/>
+      <c r="F18" s="37" t="n"/>
     </row>
     <row r="19">
       <c r="D19" s="25" t="n"/>
-      <c r="E19" s="36" t="n"/>
-      <c r="F19" s="36" t="n"/>
+      <c r="E19" s="37" t="n"/>
+      <c r="F19" s="37" t="n"/>
     </row>
     <row r="20">
       <c r="D20" s="25" t="n"/>
-      <c r="E20" s="36" t="n"/>
-      <c r="F20" s="36" t="n"/>
+      <c r="E20" s="37" t="n"/>
+      <c r="F20" s="37" t="n"/>
     </row>
     <row r="21">
       <c r="D21" s="25" t="n"/>
-      <c r="E21" s="36" t="n"/>
-      <c r="F21" s="36" t="n"/>
+      <c r="E21" s="37" t="n"/>
+      <c r="F21" s="37" t="n"/>
     </row>
     <row r="22">
       <c r="D22" s="25" t="n"/>
-      <c r="E22" s="36" t="n"/>
-      <c r="F22" s="36" t="n"/>
+      <c r="E22" s="37" t="n"/>
+      <c r="F22" s="37" t="n"/>
     </row>
     <row r="23">
       <c r="D23" s="25" t="n"/>
-      <c r="E23" s="36" t="n"/>
-      <c r="F23" s="36" t="n"/>
+      <c r="E23" s="37" t="n"/>
+      <c r="F23" s="37" t="n"/>
     </row>
     <row r="24">
       <c r="D24" s="25" t="n"/>
-      <c r="E24" s="36" t="n"/>
-      <c r="F24" s="36" t="n"/>
+      <c r="E24" s="37" t="n"/>
+      <c r="F24" s="37" t="n"/>
     </row>
     <row r="25">
       <c r="D25" s="25" t="n"/>
-      <c r="E25" s="36" t="n"/>
-      <c r="F25" s="36" t="n"/>
+      <c r="E25" s="37" t="n"/>
+      <c r="F25" s="37" t="n"/>
     </row>
     <row r="26">
       <c r="D26" s="25" t="n"/>
-      <c r="E26" s="36" t="n"/>
-      <c r="F26" s="36" t="n"/>
+      <c r="E26" s="37" t="n"/>
+      <c r="F26" s="37" t="n"/>
     </row>
     <row r="27">
       <c r="D27" s="25" t="n"/>
-      <c r="E27" s="36" t="n"/>
-      <c r="F27" s="36" t="n"/>
+      <c r="E27" s="37" t="n"/>
+      <c r="F27" s="37" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2549,7 +2555,7 @@
   </sheetPr>
   <dimension ref="D2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2557,133 +2563,133 @@
   <sheetData>
     <row r="2">
       <c r="D2" s="25" t="n"/>
-      <c r="E2" s="36" t="n"/>
-      <c r="F2" s="36" t="n"/>
+      <c r="E2" s="37" t="n"/>
+      <c r="F2" s="37" t="n"/>
     </row>
     <row r="3">
       <c r="D3" s="25" t="n"/>
-      <c r="E3" s="36" t="n"/>
-      <c r="F3" s="36" t="n"/>
+      <c r="E3" s="37" t="n"/>
+      <c r="F3" s="37" t="n"/>
     </row>
     <row r="4">
       <c r="D4" s="25" t="n"/>
-      <c r="E4" s="36" t="n"/>
-      <c r="F4" s="36" t="n"/>
+      <c r="E4" s="37" t="n"/>
+      <c r="F4" s="37" t="n"/>
     </row>
     <row r="5">
       <c r="D5" s="25" t="n"/>
-      <c r="E5" s="36" t="n"/>
-      <c r="F5" s="36" t="n"/>
+      <c r="E5" s="37" t="n"/>
+      <c r="F5" s="37" t="n"/>
     </row>
     <row r="6">
       <c r="D6" s="25" t="n"/>
-      <c r="E6" s="36" t="n"/>
-      <c r="F6" s="36" t="n"/>
+      <c r="E6" s="37" t="n"/>
+      <c r="F6" s="37" t="n"/>
     </row>
     <row r="7">
       <c r="D7" s="25" t="n"/>
-      <c r="E7" s="36" t="n"/>
-      <c r="F7" s="36" t="n"/>
+      <c r="E7" s="37" t="n"/>
+      <c r="F7" s="37" t="n"/>
     </row>
     <row r="8">
       <c r="D8" s="25" t="n"/>
-      <c r="E8" s="36" t="n"/>
-      <c r="F8" s="36" t="n"/>
+      <c r="E8" s="37" t="n"/>
+      <c r="F8" s="37" t="n"/>
     </row>
     <row r="9">
       <c r="D9" s="25" t="n"/>
-      <c r="E9" s="36" t="n"/>
-      <c r="F9" s="36" t="n"/>
+      <c r="E9" s="37" t="n"/>
+      <c r="F9" s="37" t="n"/>
     </row>
     <row r="10">
       <c r="D10" s="25" t="n"/>
-      <c r="E10" s="36" t="n"/>
-      <c r="F10" s="36" t="n"/>
+      <c r="E10" s="37" t="n"/>
+      <c r="F10" s="37" t="n"/>
     </row>
     <row r="11">
       <c r="D11" s="25" t="n"/>
-      <c r="E11" s="36" t="n"/>
-      <c r="F11" s="36" t="n"/>
+      <c r="E11" s="37" t="n"/>
+      <c r="F11" s="37" t="n"/>
     </row>
     <row r="12">
       <c r="D12" s="25" t="n"/>
-      <c r="E12" s="36" t="n"/>
-      <c r="F12" s="36" t="n"/>
+      <c r="E12" s="37" t="n"/>
+      <c r="F12" s="37" t="n"/>
     </row>
     <row r="13">
       <c r="D13" s="25" t="n"/>
-      <c r="E13" s="36" t="n"/>
-      <c r="F13" s="36" t="n"/>
+      <c r="E13" s="37" t="n"/>
+      <c r="F13" s="37" t="n"/>
     </row>
     <row r="14">
       <c r="D14" s="25" t="n"/>
-      <c r="E14" s="36" t="n"/>
-      <c r="F14" s="36" t="n"/>
+      <c r="E14" s="37" t="n"/>
+      <c r="F14" s="37" t="n"/>
     </row>
     <row r="15">
       <c r="D15" s="25" t="n"/>
-      <c r="E15" s="36" t="n"/>
-      <c r="F15" s="36" t="n"/>
+      <c r="E15" s="37" t="n"/>
+      <c r="F15" s="37" t="n"/>
     </row>
     <row r="16">
       <c r="D16" s="25" t="n"/>
-      <c r="E16" s="36" t="n"/>
-      <c r="F16" s="36" t="n"/>
+      <c r="E16" s="37" t="n"/>
+      <c r="F16" s="37" t="n"/>
     </row>
     <row r="17">
       <c r="D17" s="25" t="n"/>
-      <c r="E17" s="36" t="n"/>
-      <c r="F17" s="36" t="n"/>
+      <c r="E17" s="37" t="n"/>
+      <c r="F17" s="37" t="n"/>
     </row>
     <row r="18">
       <c r="D18" s="25" t="n"/>
-      <c r="E18" s="36" t="n"/>
-      <c r="F18" s="36" t="n"/>
+      <c r="E18" s="37" t="n"/>
+      <c r="F18" s="37" t="n"/>
     </row>
     <row r="19">
       <c r="D19" s="25" t="n"/>
-      <c r="E19" s="36" t="n"/>
-      <c r="F19" s="36" t="n"/>
+      <c r="E19" s="37" t="n"/>
+      <c r="F19" s="37" t="n"/>
     </row>
     <row r="20">
       <c r="D20" s="25" t="n"/>
-      <c r="E20" s="36" t="n"/>
-      <c r="F20" s="36" t="n"/>
+      <c r="E20" s="37" t="n"/>
+      <c r="F20" s="37" t="n"/>
     </row>
     <row r="21">
       <c r="D21" s="25" t="n"/>
-      <c r="E21" s="36" t="n"/>
-      <c r="F21" s="36" t="n"/>
+      <c r="E21" s="37" t="n"/>
+      <c r="F21" s="37" t="n"/>
     </row>
     <row r="22">
       <c r="D22" s="25" t="n"/>
-      <c r="E22" s="36" t="n"/>
-      <c r="F22" s="36" t="n"/>
+      <c r="E22" s="37" t="n"/>
+      <c r="F22" s="37" t="n"/>
     </row>
     <row r="23">
       <c r="D23" s="25" t="n"/>
-      <c r="E23" s="36" t="n"/>
-      <c r="F23" s="36" t="n"/>
+      <c r="E23" s="37" t="n"/>
+      <c r="F23" s="37" t="n"/>
     </row>
     <row r="24">
       <c r="D24" s="25" t="n"/>
-      <c r="E24" s="36" t="n"/>
-      <c r="F24" s="36" t="n"/>
+      <c r="E24" s="37" t="n"/>
+      <c r="F24" s="37" t="n"/>
     </row>
     <row r="25">
       <c r="D25" s="25" t="n"/>
-      <c r="E25" s="36" t="n"/>
-      <c r="F25" s="36" t="n"/>
+      <c r="E25" s="37" t="n"/>
+      <c r="F25" s="37" t="n"/>
     </row>
     <row r="26">
       <c r="D26" s="25" t="n"/>
-      <c r="E26" s="36" t="n"/>
-      <c r="F26" s="36" t="n"/>
+      <c r="E26" s="37" t="n"/>
+      <c r="F26" s="37" t="n"/>
     </row>
     <row r="27">
       <c r="D27" s="25" t="n"/>
-      <c r="E27" s="36" t="n"/>
-      <c r="F27" s="36" t="n"/>
+      <c r="E27" s="37" t="n"/>
+      <c r="F27" s="37" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2775,10 +2781,10 @@
       <c r="D2" s="25" t="n">
         <v>395745526</v>
       </c>
-      <c r="E2" s="39" t="n">
+      <c r="E2" s="37" t="n">
         <v>22547</v>
       </c>
-      <c r="F2" s="39" t="n">
+      <c r="F2" s="37" t="n">
         <v>44065</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -2799,128 +2805,1069 @@
     </row>
     <row r="3">
       <c r="D3" s="25" t="n"/>
-      <c r="E3" s="39" t="n"/>
-      <c r="F3" s="39" t="n"/>
+      <c r="E3" s="37" t="n"/>
+      <c r="F3" s="37" t="n"/>
     </row>
     <row r="4">
       <c r="D4" s="25" t="n"/>
-      <c r="E4" s="39" t="n"/>
-      <c r="F4" s="39" t="n"/>
+      <c r="E4" s="37" t="n"/>
+      <c r="F4" s="37" t="n"/>
     </row>
     <row r="5">
       <c r="D5" s="25" t="n"/>
-      <c r="E5" s="39" t="n"/>
-      <c r="F5" s="39" t="n"/>
+      <c r="E5" s="37" t="n"/>
+      <c r="F5" s="37" t="n"/>
     </row>
     <row r="6">
       <c r="D6" s="25" t="n"/>
-      <c r="E6" s="39" t="n"/>
-      <c r="F6" s="39" t="n"/>
+      <c r="E6" s="37" t="n"/>
+      <c r="F6" s="37" t="n"/>
     </row>
     <row r="7">
       <c r="D7" s="25" t="n"/>
-      <c r="E7" s="39" t="n"/>
-      <c r="F7" s="39" t="n"/>
+      <c r="E7" s="37" t="n"/>
+      <c r="F7" s="37" t="n"/>
     </row>
     <row r="8">
       <c r="D8" s="25" t="n"/>
-      <c r="E8" s="39" t="n"/>
-      <c r="F8" s="39" t="n"/>
+      <c r="E8" s="37" t="n"/>
+      <c r="F8" s="37" t="n"/>
     </row>
     <row r="9">
       <c r="D9" s="25" t="n"/>
-      <c r="E9" s="39" t="n"/>
-      <c r="F9" s="39" t="n"/>
+      <c r="E9" s="37" t="n"/>
+      <c r="F9" s="37" t="n"/>
     </row>
     <row r="10">
       <c r="D10" s="25" t="n"/>
-      <c r="E10" s="39" t="n"/>
-      <c r="F10" s="39" t="n"/>
+      <c r="E10" s="37" t="n"/>
+      <c r="F10" s="37" t="n"/>
     </row>
     <row r="11">
       <c r="D11" s="25" t="n"/>
-      <c r="E11" s="39" t="n"/>
-      <c r="F11" s="39" t="n"/>
+      <c r="E11" s="37" t="n"/>
+      <c r="F11" s="37" t="n"/>
     </row>
     <row r="12">
       <c r="D12" s="25" t="n"/>
-      <c r="E12" s="39" t="n"/>
-      <c r="F12" s="39" t="n"/>
+      <c r="E12" s="37" t="n"/>
+      <c r="F12" s="37" t="n"/>
     </row>
     <row r="13">
       <c r="D13" s="25" t="n"/>
-      <c r="E13" s="39" t="n"/>
-      <c r="F13" s="39" t="n"/>
+      <c r="E13" s="37" t="n"/>
+      <c r="F13" s="37" t="n"/>
     </row>
     <row r="14">
       <c r="D14" s="25" t="n"/>
-      <c r="E14" s="39" t="n"/>
-      <c r="F14" s="39" t="n"/>
+      <c r="E14" s="37" t="n"/>
+      <c r="F14" s="37" t="n"/>
     </row>
     <row r="15">
       <c r="D15" s="25" t="n"/>
-      <c r="E15" s="39" t="n"/>
-      <c r="F15" s="39" t="n"/>
+      <c r="E15" s="37" t="n"/>
+      <c r="F15" s="37" t="n"/>
     </row>
     <row r="16">
       <c r="D16" s="25" t="n"/>
-      <c r="E16" s="39" t="n"/>
-      <c r="F16" s="39" t="n"/>
+      <c r="E16" s="37" t="n"/>
+      <c r="F16" s="37" t="n"/>
     </row>
     <row r="17">
       <c r="D17" s="25" t="n"/>
-      <c r="E17" s="39" t="n"/>
-      <c r="F17" s="39" t="n"/>
+      <c r="E17" s="37" t="n"/>
+      <c r="F17" s="37" t="n"/>
     </row>
     <row r="18">
       <c r="D18" s="25" t="n"/>
-      <c r="E18" s="39" t="n"/>
-      <c r="F18" s="39" t="n"/>
+      <c r="E18" s="37" t="n"/>
+      <c r="F18" s="37" t="n"/>
     </row>
     <row r="19">
       <c r="D19" s="25" t="n"/>
-      <c r="E19" s="39" t="n"/>
-      <c r="F19" s="39" t="n"/>
+      <c r="E19" s="37" t="n"/>
+      <c r="F19" s="37" t="n"/>
     </row>
     <row r="20">
       <c r="D20" s="25" t="n"/>
-      <c r="E20" s="39" t="n"/>
-      <c r="F20" s="39" t="n"/>
+      <c r="E20" s="37" t="n"/>
+      <c r="F20" s="37" t="n"/>
     </row>
     <row r="21">
       <c r="D21" s="25" t="n"/>
-      <c r="E21" s="39" t="n"/>
-      <c r="F21" s="39" t="n"/>
+      <c r="E21" s="37" t="n"/>
+      <c r="F21" s="37" t="n"/>
     </row>
     <row r="22">
       <c r="D22" s="25" t="n"/>
-      <c r="E22" s="39" t="n"/>
-      <c r="F22" s="39" t="n"/>
+      <c r="E22" s="37" t="n"/>
+      <c r="F22" s="37" t="n"/>
     </row>
     <row r="23">
       <c r="D23" s="25" t="n"/>
-      <c r="E23" s="39" t="n"/>
-      <c r="F23" s="39" t="n"/>
+      <c r="E23" s="37" t="n"/>
+      <c r="F23" s="37" t="n"/>
     </row>
     <row r="24">
       <c r="D24" s="25" t="n"/>
-      <c r="E24" s="39" t="n"/>
-      <c r="F24" s="39" t="n"/>
+      <c r="E24" s="37" t="n"/>
+      <c r="F24" s="37" t="n"/>
     </row>
     <row r="25">
       <c r="D25" s="25" t="n"/>
-      <c r="E25" s="39" t="n"/>
-      <c r="F25" s="39" t="n"/>
+      <c r="E25" s="37" t="n"/>
+      <c r="F25" s="37" t="n"/>
     </row>
     <row r="26">
       <c r="D26" s="25" t="n"/>
-      <c r="E26" s="39" t="n"/>
-      <c r="F26" s="39" t="n"/>
+      <c r="E26" s="37" t="n"/>
+      <c r="F26" s="37" t="n"/>
     </row>
     <row r="27">
       <c r="D27" s="25" t="n"/>
-      <c r="E27" s="39" t="n"/>
-      <c r="F27" s="39" t="n"/>
+      <c r="E27" s="37" t="n"/>
+      <c r="F27" s="37" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Firstname</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Lastname</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Birth date</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Test date</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Patient Status</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Quarantined</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Where quarantined</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Tesed</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D2" s="25" t="n">
+        <v>24314412</v>
+      </c>
+      <c r="E2" s="37" t="n">
+        <v>24720</v>
+      </c>
+      <c r="F2" s="37" t="n">
+        <v>44510</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" s="25" t="n"/>
+      <c r="E3" s="37" t="n"/>
+      <c r="F3" s="37" t="n"/>
+    </row>
+    <row r="4">
+      <c r="D4" s="25" t="n"/>
+      <c r="E4" s="37" t="n"/>
+      <c r="F4" s="37" t="n"/>
+    </row>
+    <row r="5">
+      <c r="D5" s="25" t="n"/>
+      <c r="E5" s="37" t="n"/>
+      <c r="F5" s="37" t="n"/>
+    </row>
+    <row r="6">
+      <c r="D6" s="25" t="n"/>
+      <c r="E6" s="37" t="n"/>
+      <c r="F6" s="37" t="n"/>
+    </row>
+    <row r="7">
+      <c r="D7" s="25" t="n"/>
+      <c r="E7" s="37" t="n"/>
+      <c r="F7" s="37" t="n"/>
+    </row>
+    <row r="8">
+      <c r="D8" s="25" t="n"/>
+      <c r="E8" s="37" t="n"/>
+      <c r="F8" s="37" t="n"/>
+    </row>
+    <row r="9">
+      <c r="D9" s="25" t="n"/>
+      <c r="E9" s="37" t="n"/>
+      <c r="F9" s="37" t="n"/>
+    </row>
+    <row r="10">
+      <c r="D10" s="25" t="n"/>
+      <c r="E10" s="37" t="n"/>
+      <c r="F10" s="37" t="n"/>
+    </row>
+    <row r="11">
+      <c r="D11" s="25" t="n"/>
+      <c r="E11" s="37" t="n"/>
+      <c r="F11" s="37" t="n"/>
+    </row>
+    <row r="12">
+      <c r="D12" s="25" t="n"/>
+      <c r="E12" s="37" t="n"/>
+      <c r="F12" s="37" t="n"/>
+    </row>
+    <row r="13">
+      <c r="D13" s="25" t="n"/>
+      <c r="E13" s="37" t="n"/>
+      <c r="F13" s="37" t="n"/>
+    </row>
+    <row r="14">
+      <c r="D14" s="25" t="n"/>
+      <c r="E14" s="37" t="n"/>
+      <c r="F14" s="37" t="n"/>
+    </row>
+    <row r="15">
+      <c r="D15" s="25" t="n"/>
+      <c r="E15" s="37" t="n"/>
+      <c r="F15" s="37" t="n"/>
+    </row>
+    <row r="16">
+      <c r="D16" s="25" t="n"/>
+      <c r="E16" s="37" t="n"/>
+      <c r="F16" s="37" t="n"/>
+    </row>
+    <row r="17">
+      <c r="D17" s="25" t="n"/>
+      <c r="E17" s="37" t="n"/>
+      <c r="F17" s="37" t="n"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="25" t="n"/>
+      <c r="E18" s="37" t="n"/>
+      <c r="F18" s="37" t="n"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="25" t="n"/>
+      <c r="E19" s="37" t="n"/>
+      <c r="F19" s="37" t="n"/>
+    </row>
+    <row r="20">
+      <c r="D20" s="25" t="n"/>
+      <c r="E20" s="37" t="n"/>
+      <c r="F20" s="37" t="n"/>
+    </row>
+    <row r="21">
+      <c r="D21" s="25" t="n"/>
+      <c r="E21" s="37" t="n"/>
+      <c r="F21" s="37" t="n"/>
+    </row>
+    <row r="22">
+      <c r="D22" s="25" t="n"/>
+      <c r="E22" s="37" t="n"/>
+      <c r="F22" s="37" t="n"/>
+    </row>
+    <row r="23">
+      <c r="D23" s="25" t="n"/>
+      <c r="E23" s="37" t="n"/>
+      <c r="F23" s="37" t="n"/>
+    </row>
+    <row r="24">
+      <c r="D24" s="25" t="n"/>
+      <c r="E24" s="37" t="n"/>
+      <c r="F24" s="37" t="n"/>
+    </row>
+    <row r="25">
+      <c r="D25" s="25" t="n"/>
+      <c r="E25" s="37" t="n"/>
+      <c r="F25" s="37" t="n"/>
+    </row>
+    <row r="26">
+      <c r="D26" s="25" t="n"/>
+      <c r="E26" s="37" t="n"/>
+      <c r="F26" s="37" t="n"/>
+    </row>
+    <row r="27">
+      <c r="D27" s="25" t="n"/>
+      <c r="E27" s="37" t="n"/>
+      <c r="F27" s="37" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Firstname</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Lastname</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Occupation</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Birth date</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Test date</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Patient Status</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Quarantined</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Where quarantined</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Dsadafsa</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dfhgsdgf</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D2" s="25" t="n">
+        <v>34252353</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Azmaiiasdf</t>
+        </is>
+      </c>
+      <c r="F2" s="37" t="n">
+        <v>15987</v>
+      </c>
+      <c r="G2" s="35" t="n">
+        <v>43709</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Hospital</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" s="25" t="n"/>
+      <c r="F3" s="37" t="n"/>
+    </row>
+    <row r="4">
+      <c r="D4" s="25" t="n"/>
+      <c r="F4" s="37" t="n"/>
+    </row>
+    <row r="5">
+      <c r="D5" s="25" t="n"/>
+      <c r="F5" s="37" t="n"/>
+    </row>
+    <row r="6">
+      <c r="D6" s="25" t="n"/>
+      <c r="F6" s="37" t="n"/>
+    </row>
+    <row r="7">
+      <c r="D7" s="25" t="n"/>
+      <c r="F7" s="37" t="n"/>
+    </row>
+    <row r="8">
+      <c r="D8" s="25" t="n"/>
+      <c r="F8" s="37" t="n"/>
+    </row>
+    <row r="9">
+      <c r="D9" s="25" t="n"/>
+      <c r="F9" s="37" t="n"/>
+    </row>
+    <row r="10">
+      <c r="D10" s="25" t="n"/>
+      <c r="F10" s="37" t="n"/>
+    </row>
+    <row r="11">
+      <c r="D11" s="25" t="n"/>
+      <c r="F11" s="37" t="n"/>
+    </row>
+    <row r="12">
+      <c r="D12" s="25" t="n"/>
+      <c r="F12" s="37" t="n"/>
+    </row>
+    <row r="13">
+      <c r="D13" s="25" t="n"/>
+      <c r="F13" s="37" t="n"/>
+    </row>
+    <row r="14">
+      <c r="D14" s="25" t="n"/>
+      <c r="F14" s="37" t="n"/>
+    </row>
+    <row r="15">
+      <c r="D15" s="25" t="n"/>
+      <c r="F15" s="37" t="n"/>
+    </row>
+    <row r="16">
+      <c r="D16" s="25" t="n"/>
+      <c r="F16" s="37" t="n"/>
+    </row>
+    <row r="17">
+      <c r="D17" s="25" t="n"/>
+      <c r="F17" s="37" t="n"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="25" t="n"/>
+      <c r="F18" s="37" t="n"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="25" t="n"/>
+      <c r="F19" s="37" t="n"/>
+    </row>
+    <row r="20">
+      <c r="D20" s="25" t="n"/>
+      <c r="F20" s="37" t="n"/>
+    </row>
+    <row r="21">
+      <c r="D21" s="25" t="n"/>
+      <c r="F21" s="37" t="n"/>
+    </row>
+    <row r="22">
+      <c r="D22" s="25" t="n"/>
+      <c r="F22" s="37" t="n"/>
+    </row>
+    <row r="23">
+      <c r="D23" s="25" t="n"/>
+      <c r="F23" s="37" t="n"/>
+    </row>
+    <row r="24">
+      <c r="D24" s="25" t="n"/>
+      <c r="F24" s="37" t="n"/>
+    </row>
+    <row r="25">
+      <c r="D25" s="25" t="n"/>
+      <c r="F25" s="37" t="n"/>
+    </row>
+    <row r="26">
+      <c r="D26" s="25" t="n"/>
+      <c r="F26" s="37" t="n"/>
+    </row>
+    <row r="27">
+      <c r="D27" s="25" t="n"/>
+      <c r="F27" s="37" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Firstname</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Lastname</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Occupation</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Birth date</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Test date</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Patient Status</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Quarantined</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Where quarantined</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fafasf</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>fasfasf</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D2" s="25" t="n">
+        <v>214415415</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>School Student</t>
+        </is>
+      </c>
+      <c r="F2" s="37" t="n">
+        <v>29132</v>
+      </c>
+      <c r="G2" s="35" t="n">
+        <v>44145</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>sdfFDS@gasjn.safda</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" s="25" t="n"/>
+      <c r="F3" s="37" t="n"/>
+    </row>
+    <row r="4">
+      <c r="D4" s="25" t="n"/>
+      <c r="F4" s="37" t="n"/>
+    </row>
+    <row r="5">
+      <c r="D5" s="25" t="n"/>
+      <c r="F5" s="37" t="n"/>
+    </row>
+    <row r="6">
+      <c r="D6" s="25" t="n"/>
+      <c r="F6" s="37" t="n"/>
+    </row>
+    <row r="7">
+      <c r="D7" s="25" t="n"/>
+      <c r="F7" s="37" t="n"/>
+    </row>
+    <row r="8">
+      <c r="D8" s="25" t="n"/>
+      <c r="F8" s="37" t="n"/>
+    </row>
+    <row r="9">
+      <c r="D9" s="25" t="n"/>
+      <c r="F9" s="37" t="n"/>
+    </row>
+    <row r="10">
+      <c r="D10" s="25" t="n"/>
+      <c r="F10" s="37" t="n"/>
+    </row>
+    <row r="11">
+      <c r="D11" s="25" t="n"/>
+      <c r="F11" s="37" t="n"/>
+    </row>
+    <row r="12">
+      <c r="D12" s="25" t="n"/>
+      <c r="F12" s="37" t="n"/>
+    </row>
+    <row r="13">
+      <c r="D13" s="25" t="n"/>
+      <c r="F13" s="37" t="n"/>
+    </row>
+    <row r="14">
+      <c r="D14" s="25" t="n"/>
+      <c r="F14" s="37" t="n"/>
+    </row>
+    <row r="15">
+      <c r="D15" s="25" t="n"/>
+      <c r="F15" s="37" t="n"/>
+    </row>
+    <row r="16">
+      <c r="D16" s="25" t="n"/>
+      <c r="F16" s="37" t="n"/>
+    </row>
+    <row r="17">
+      <c r="D17" s="25" t="n"/>
+      <c r="F17" s="37" t="n"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="25" t="n"/>
+      <c r="F18" s="37" t="n"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="25" t="n"/>
+      <c r="F19" s="37" t="n"/>
+    </row>
+    <row r="20">
+      <c r="D20" s="25" t="n"/>
+      <c r="F20" s="37" t="n"/>
+    </row>
+    <row r="21">
+      <c r="D21" s="25" t="n"/>
+      <c r="F21" s="37" t="n"/>
+    </row>
+    <row r="22">
+      <c r="D22" s="25" t="n"/>
+      <c r="F22" s="37" t="n"/>
+    </row>
+    <row r="23">
+      <c r="D23" s="25" t="n"/>
+      <c r="F23" s="37" t="n"/>
+    </row>
+    <row r="24">
+      <c r="D24" s="25" t="n"/>
+      <c r="F24" s="37" t="n"/>
+    </row>
+    <row r="25">
+      <c r="D25" s="25" t="n"/>
+      <c r="F25" s="37" t="n"/>
+    </row>
+    <row r="26">
+      <c r="D26" s="25" t="n"/>
+      <c r="F26" s="37" t="n"/>
+    </row>
+    <row r="27">
+      <c r="D27" s="25" t="n"/>
+      <c r="F27" s="37" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Firstname</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Lastname</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Occupation</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Birth date</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Test date</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Patient Status</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Quarantined</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Where quarantined</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fafdfh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dfghfdgh</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D2" s="25" t="n">
+        <v>41241241</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pensioner</t>
+        </is>
+      </c>
+      <c r="F2" s="38" t="n">
+        <v>7253</v>
+      </c>
+      <c r="G2" s="39" t="n">
+        <v>44371</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Hotel</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>ds@sdasd.asff</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" s="25" t="n"/>
+      <c r="F3" s="38" t="n"/>
+    </row>
+    <row r="4">
+      <c r="D4" s="25" t="n"/>
+      <c r="F4" s="38" t="n"/>
+    </row>
+    <row r="5">
+      <c r="D5" s="25" t="n"/>
+      <c r="F5" s="38" t="n"/>
+    </row>
+    <row r="6">
+      <c r="D6" s="25" t="n"/>
+      <c r="F6" s="38" t="n"/>
+    </row>
+    <row r="7">
+      <c r="D7" s="25" t="n"/>
+      <c r="F7" s="38" t="n"/>
+    </row>
+    <row r="8">
+      <c r="D8" s="25" t="n"/>
+      <c r="F8" s="38" t="n"/>
+    </row>
+    <row r="9">
+      <c r="D9" s="25" t="n"/>
+      <c r="F9" s="38" t="n"/>
+    </row>
+    <row r="10">
+      <c r="D10" s="25" t="n"/>
+      <c r="F10" s="38" t="n"/>
+    </row>
+    <row r="11">
+      <c r="D11" s="25" t="n"/>
+      <c r="F11" s="38" t="n"/>
+    </row>
+    <row r="12">
+      <c r="D12" s="25" t="n"/>
+      <c r="F12" s="38" t="n"/>
+    </row>
+    <row r="13">
+      <c r="D13" s="25" t="n"/>
+      <c r="F13" s="38" t="n"/>
+    </row>
+    <row r="14">
+      <c r="D14" s="25" t="n"/>
+      <c r="F14" s="38" t="n"/>
+    </row>
+    <row r="15">
+      <c r="D15" s="25" t="n"/>
+      <c r="F15" s="38" t="n"/>
+    </row>
+    <row r="16">
+      <c r="D16" s="25" t="n"/>
+      <c r="F16" s="38" t="n"/>
+    </row>
+    <row r="17">
+      <c r="D17" s="25" t="n"/>
+      <c r="F17" s="38" t="n"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="25" t="n"/>
+      <c r="F18" s="38" t="n"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="25" t="n"/>
+      <c r="F19" s="38" t="n"/>
+    </row>
+    <row r="20">
+      <c r="D20" s="25" t="n"/>
+      <c r="F20" s="38" t="n"/>
+    </row>
+    <row r="21">
+      <c r="D21" s="25" t="n"/>
+      <c r="F21" s="38" t="n"/>
+    </row>
+    <row r="22">
+      <c r="D22" s="25" t="n"/>
+      <c r="F22" s="38" t="n"/>
+    </row>
+    <row r="23">
+      <c r="D23" s="25" t="n"/>
+      <c r="F23" s="38" t="n"/>
+    </row>
+    <row r="24">
+      <c r="D24" s="25" t="n"/>
+      <c r="F24" s="38" t="n"/>
+    </row>
+    <row r="25">
+      <c r="D25" s="25" t="n"/>
+      <c r="F25" s="38" t="n"/>
+    </row>
+    <row r="26">
+      <c r="D26" s="25" t="n"/>
+      <c r="F26" s="38" t="n"/>
+    </row>
+    <row r="27">
+      <c r="D27" s="25" t="n"/>
+      <c r="F27" s="38" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -3029,7 +3976,7 @@
       <c r="E2" s="22" t="n">
         <v>35028</v>
       </c>
-      <c r="F2" s="32" t="n">
+      <c r="F2" s="36" t="n">
         <v>44037</v>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -3070,7 +4017,7 @@
       <c r="E3" s="22" t="n">
         <v>35028</v>
       </c>
-      <c r="F3" s="32" t="n">
+      <c r="F3" s="36" t="n">
         <v>44037</v>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -3111,7 +4058,7 @@
       <c r="E4" s="22" t="n">
         <v>6793</v>
       </c>
-      <c r="F4" s="32" t="n">
+      <c r="F4" s="36" t="n">
         <v>44019</v>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -3152,7 +4099,7 @@
       <c r="E5" s="22" t="n">
         <v>20704</v>
       </c>
-      <c r="F5" s="32" t="n">
+      <c r="F5" s="36" t="n">
         <v>44113</v>
       </c>
       <c r="G5" s="1" t="inlineStr">
@@ -3193,7 +4140,7 @@
       <c r="E6" s="22" t="n">
         <v>30681</v>
       </c>
-      <c r="F6" s="32" t="n">
+      <c r="F6" s="36" t="n">
         <v>43592</v>
       </c>
       <c r="G6" s="1" t="inlineStr">
@@ -3234,7 +4181,7 @@
       <c r="E7" s="22" t="n">
         <v>35285</v>
       </c>
-      <c r="F7" s="32" t="n">
+      <c r="F7" s="36" t="n">
         <v>43990</v>
       </c>
       <c r="G7" s="1" t="inlineStr">
@@ -3275,7 +4222,7 @@
       <c r="E8" s="22" t="n">
         <v>35285</v>
       </c>
-      <c r="F8" s="32" t="n">
+      <c r="F8" s="36" t="n">
         <v>43990</v>
       </c>
       <c r="G8" s="1" t="inlineStr">
@@ -3316,7 +4263,7 @@
       <c r="E9" s="22" t="n">
         <v>12274</v>
       </c>
-      <c r="F9" s="35" t="n">
+      <c r="F9" s="30" t="n">
         <v>44355</v>
       </c>
       <c r="G9" s="1" t="inlineStr">
@@ -3357,7 +4304,7 @@
       <c r="E10" s="22" t="n">
         <v>8024</v>
       </c>
-      <c r="F10" s="35" t="n">
+      <c r="F10" s="30" t="n">
         <v>44021</v>
       </c>
       <c r="G10" s="1" t="inlineStr">
@@ -4451,10 +5398,10 @@
       <c r="D2" s="25" t="n">
         <v>154215123</v>
       </c>
-      <c r="E2" s="36" t="n">
+      <c r="E2" s="37" t="n">
         <v>7953</v>
       </c>
-      <c r="F2" s="36" t="n">
+      <c r="F2" s="37" t="n">
         <v>44168</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -4470,128 +5417,128 @@
     </row>
     <row r="3">
       <c r="D3" s="25" t="n"/>
-      <c r="E3" s="36" t="n"/>
-      <c r="F3" s="36" t="n"/>
+      <c r="E3" s="37" t="n"/>
+      <c r="F3" s="37" t="n"/>
     </row>
     <row r="4">
       <c r="D4" s="25" t="n"/>
-      <c r="E4" s="36" t="n"/>
-      <c r="F4" s="36" t="n"/>
+      <c r="E4" s="37" t="n"/>
+      <c r="F4" s="37" t="n"/>
     </row>
     <row r="5">
       <c r="D5" s="25" t="n"/>
-      <c r="E5" s="36" t="n"/>
-      <c r="F5" s="36" t="n"/>
+      <c r="E5" s="37" t="n"/>
+      <c r="F5" s="37" t="n"/>
     </row>
     <row r="6">
       <c r="D6" s="25" t="n"/>
-      <c r="E6" s="36" t="n"/>
-      <c r="F6" s="36" t="n"/>
+      <c r="E6" s="37" t="n"/>
+      <c r="F6" s="37" t="n"/>
     </row>
     <row r="7">
       <c r="D7" s="25" t="n"/>
-      <c r="E7" s="36" t="n"/>
-      <c r="F7" s="36" t="n"/>
+      <c r="E7" s="37" t="n"/>
+      <c r="F7" s="37" t="n"/>
     </row>
     <row r="8">
       <c r="D8" s="25" t="n"/>
-      <c r="E8" s="36" t="n"/>
-      <c r="F8" s="36" t="n"/>
+      <c r="E8" s="37" t="n"/>
+      <c r="F8" s="37" t="n"/>
     </row>
     <row r="9">
       <c r="D9" s="25" t="n"/>
-      <c r="E9" s="36" t="n"/>
-      <c r="F9" s="36" t="n"/>
+      <c r="E9" s="37" t="n"/>
+      <c r="F9" s="37" t="n"/>
     </row>
     <row r="10">
       <c r="D10" s="25" t="n"/>
-      <c r="E10" s="36" t="n"/>
-      <c r="F10" s="36" t="n"/>
+      <c r="E10" s="37" t="n"/>
+      <c r="F10" s="37" t="n"/>
     </row>
     <row r="11">
       <c r="D11" s="25" t="n"/>
-      <c r="E11" s="36" t="n"/>
-      <c r="F11" s="36" t="n"/>
+      <c r="E11" s="37" t="n"/>
+      <c r="F11" s="37" t="n"/>
     </row>
     <row r="12">
       <c r="D12" s="25" t="n"/>
-      <c r="E12" s="36" t="n"/>
-      <c r="F12" s="36" t="n"/>
+      <c r="E12" s="37" t="n"/>
+      <c r="F12" s="37" t="n"/>
     </row>
     <row r="13">
       <c r="D13" s="25" t="n"/>
-      <c r="E13" s="36" t="n"/>
-      <c r="F13" s="36" t="n"/>
+      <c r="E13" s="37" t="n"/>
+      <c r="F13" s="37" t="n"/>
     </row>
     <row r="14">
       <c r="D14" s="25" t="n"/>
-      <c r="E14" s="36" t="n"/>
-      <c r="F14" s="36" t="n"/>
+      <c r="E14" s="37" t="n"/>
+      <c r="F14" s="37" t="n"/>
     </row>
     <row r="15">
       <c r="D15" s="25" t="n"/>
-      <c r="E15" s="36" t="n"/>
-      <c r="F15" s="36" t="n"/>
+      <c r="E15" s="37" t="n"/>
+      <c r="F15" s="37" t="n"/>
     </row>
     <row r="16">
       <c r="D16" s="25" t="n"/>
-      <c r="E16" s="36" t="n"/>
-      <c r="F16" s="36" t="n"/>
+      <c r="E16" s="37" t="n"/>
+      <c r="F16" s="37" t="n"/>
     </row>
     <row r="17">
       <c r="D17" s="25" t="n"/>
-      <c r="E17" s="36" t="n"/>
-      <c r="F17" s="36" t="n"/>
+      <c r="E17" s="37" t="n"/>
+      <c r="F17" s="37" t="n"/>
     </row>
     <row r="18">
       <c r="D18" s="25" t="n"/>
-      <c r="E18" s="36" t="n"/>
-      <c r="F18" s="36" t="n"/>
+      <c r="E18" s="37" t="n"/>
+      <c r="F18" s="37" t="n"/>
     </row>
     <row r="19">
       <c r="D19" s="25" t="n"/>
-      <c r="E19" s="36" t="n"/>
-      <c r="F19" s="36" t="n"/>
+      <c r="E19" s="37" t="n"/>
+      <c r="F19" s="37" t="n"/>
     </row>
     <row r="20">
       <c r="D20" s="25" t="n"/>
-      <c r="E20" s="36" t="n"/>
-      <c r="F20" s="36" t="n"/>
+      <c r="E20" s="37" t="n"/>
+      <c r="F20" s="37" t="n"/>
     </row>
     <row r="21">
       <c r="D21" s="25" t="n"/>
-      <c r="E21" s="36" t="n"/>
-      <c r="F21" s="36" t="n"/>
+      <c r="E21" s="37" t="n"/>
+      <c r="F21" s="37" t="n"/>
     </row>
     <row r="22">
       <c r="D22" s="25" t="n"/>
-      <c r="E22" s="36" t="n"/>
-      <c r="F22" s="36" t="n"/>
+      <c r="E22" s="37" t="n"/>
+      <c r="F22" s="37" t="n"/>
     </row>
     <row r="23">
       <c r="D23" s="25" t="n"/>
-      <c r="E23" s="36" t="n"/>
-      <c r="F23" s="36" t="n"/>
+      <c r="E23" s="37" t="n"/>
+      <c r="F23" s="37" t="n"/>
     </row>
     <row r="24">
       <c r="D24" s="25" t="n"/>
-      <c r="E24" s="36" t="n"/>
-      <c r="F24" s="36" t="n"/>
+      <c r="E24" s="37" t="n"/>
+      <c r="F24" s="37" t="n"/>
     </row>
     <row r="25">
       <c r="D25" s="25" t="n"/>
-      <c r="E25" s="36" t="n"/>
-      <c r="F25" s="36" t="n"/>
+      <c r="E25" s="37" t="n"/>
+      <c r="F25" s="37" t="n"/>
     </row>
     <row r="26">
       <c r="D26" s="25" t="n"/>
-      <c r="E26" s="36" t="n"/>
-      <c r="F26" s="36" t="n"/>
+      <c r="E26" s="37" t="n"/>
+      <c r="F26" s="37" t="n"/>
     </row>
     <row r="27">
       <c r="D27" s="25" t="n"/>
-      <c r="E27" s="36" t="n"/>
-      <c r="F27" s="36" t="n"/>
+      <c r="E27" s="37" t="n"/>
+      <c r="F27" s="37" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -4692,10 +5639,10 @@
       <c r="D2" s="28" t="n">
         <v>544327551</v>
       </c>
-      <c r="E2" s="37" t="n">
+      <c r="E2" s="32" t="n">
         <v>36020</v>
       </c>
-      <c r="F2" s="38" t="n">
+      <c r="F2" s="35" t="n">
         <v>44037</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -4733,10 +5680,10 @@
       <c r="D3" s="28" t="n">
         <v>320620321</v>
       </c>
-      <c r="E3" s="37" t="n">
+      <c r="E3" s="32" t="n">
         <v>35046</v>
       </c>
-      <c r="F3" s="38" t="n">
+      <c r="F3" s="35" t="n">
         <v>43987</v>
       </c>
       <c r="G3" t="inlineStr">
@@ -4775,10 +5722,10 @@
       <c r="D4" s="28" t="n">
         <v>123456789</v>
       </c>
-      <c r="E4" s="37" t="n">
+      <c r="E4" s="32" t="n">
         <v>35046</v>
       </c>
-      <c r="F4" s="38" t="n">
+      <c r="F4" s="35" t="n">
         <v>43988</v>
       </c>
       <c r="G4" t="inlineStr">
@@ -4816,10 +5763,10 @@
       <c r="D5" s="28" t="n">
         <v>452635847</v>
       </c>
-      <c r="E5" s="37" t="n">
+      <c r="E5" s="32" t="n">
         <v>35046</v>
       </c>
-      <c r="F5" s="38" t="n">
+      <c r="F5" s="35" t="n">
         <v>44384</v>
       </c>
       <c r="G5" t="inlineStr">
@@ -4857,10 +5804,10 @@
       <c r="D6" s="28" t="n">
         <v>852455951</v>
       </c>
-      <c r="E6" s="37" t="n">
+      <c r="E6" s="32" t="n">
         <v>12702</v>
       </c>
-      <c r="F6" s="38" t="n">
+      <c r="F6" s="35" t="n">
         <v>44366</v>
       </c>
       <c r="G6" t="inlineStr">
@@ -4898,10 +5845,10 @@
       <c r="D7" s="28" t="n">
         <v>235463765</v>
       </c>
-      <c r="E7" s="37" t="n">
+      <c r="E7" s="32" t="n">
         <v>8318</v>
       </c>
-      <c r="F7" s="38" t="n">
+      <c r="F7" s="35" t="n">
         <v>44009</v>
       </c>
       <c r="G7" t="inlineStr">
@@ -4922,39 +5869,39 @@
     </row>
     <row r="8">
       <c r="D8" s="28" t="n"/>
-      <c r="E8" s="37" t="n"/>
+      <c r="E8" s="32" t="n"/>
     </row>
     <row r="9">
       <c r="D9" s="28" t="n"/>
-      <c r="E9" s="37" t="n"/>
+      <c r="E9" s="32" t="n"/>
     </row>
     <row r="10">
       <c r="D10" s="28" t="n"/>
-      <c r="E10" s="37" t="n"/>
+      <c r="E10" s="32" t="n"/>
     </row>
     <row r="11">
       <c r="D11" s="28" t="n"/>
-      <c r="E11" s="37" t="n"/>
+      <c r="E11" s="32" t="n"/>
     </row>
     <row r="12">
       <c r="D12" s="28" t="n"/>
-      <c r="E12" s="37" t="n"/>
+      <c r="E12" s="32" t="n"/>
     </row>
     <row r="13">
       <c r="D13" s="28" t="n"/>
-      <c r="E13" s="37" t="n"/>
+      <c r="E13" s="32" t="n"/>
     </row>
     <row r="14">
       <c r="D14" s="28" t="n"/>
-      <c r="E14" s="37" t="n"/>
+      <c r="E14" s="32" t="n"/>
     </row>
     <row r="15">
       <c r="D15" s="28" t="n"/>
-      <c r="E15" s="37" t="n"/>
+      <c r="E15" s="32" t="n"/>
     </row>
     <row r="16">
       <c r="D16" s="28" t="n"/>
-      <c r="E16" s="37" t="n"/>
+      <c r="E16" s="32" t="n"/>
     </row>
     <row r="17">
       <c r="D17" s="28" t="n"/>
@@ -5106,10 +6053,10 @@
       <c r="D2" s="25" t="n">
         <v>235624857</v>
       </c>
-      <c r="E2" s="36" t="n">
+      <c r="E2" s="37" t="n">
         <v>29186</v>
       </c>
-      <c r="F2" s="36" t="n">
+      <c r="F2" s="37" t="n">
         <v>43928</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -5130,128 +6077,128 @@
     </row>
     <row r="3">
       <c r="D3" s="25" t="n"/>
-      <c r="E3" s="36" t="n"/>
-      <c r="F3" s="36" t="n"/>
+      <c r="E3" s="37" t="n"/>
+      <c r="F3" s="37" t="n"/>
     </row>
     <row r="4">
       <c r="D4" s="25" t="n"/>
-      <c r="E4" s="36" t="n"/>
-      <c r="F4" s="36" t="n"/>
+      <c r="E4" s="37" t="n"/>
+      <c r="F4" s="37" t="n"/>
     </row>
     <row r="5">
       <c r="D5" s="25" t="n"/>
-      <c r="E5" s="36" t="n"/>
-      <c r="F5" s="36" t="n"/>
+      <c r="E5" s="37" t="n"/>
+      <c r="F5" s="37" t="n"/>
     </row>
     <row r="6">
       <c r="D6" s="25" t="n"/>
-      <c r="E6" s="36" t="n"/>
-      <c r="F6" s="36" t="n"/>
+      <c r="E6" s="37" t="n"/>
+      <c r="F6" s="37" t="n"/>
     </row>
     <row r="7">
       <c r="D7" s="25" t="n"/>
-      <c r="E7" s="36" t="n"/>
-      <c r="F7" s="36" t="n"/>
+      <c r="E7" s="37" t="n"/>
+      <c r="F7" s="37" t="n"/>
     </row>
     <row r="8">
       <c r="D8" s="25" t="n"/>
-      <c r="E8" s="36" t="n"/>
-      <c r="F8" s="36" t="n"/>
+      <c r="E8" s="37" t="n"/>
+      <c r="F8" s="37" t="n"/>
     </row>
     <row r="9">
       <c r="D9" s="25" t="n"/>
-      <c r="E9" s="36" t="n"/>
-      <c r="F9" s="36" t="n"/>
+      <c r="E9" s="37" t="n"/>
+      <c r="F9" s="37" t="n"/>
     </row>
     <row r="10">
       <c r="D10" s="25" t="n"/>
-      <c r="E10" s="36" t="n"/>
-      <c r="F10" s="36" t="n"/>
+      <c r="E10" s="37" t="n"/>
+      <c r="F10" s="37" t="n"/>
     </row>
     <row r="11">
       <c r="D11" s="25" t="n"/>
-      <c r="E11" s="36" t="n"/>
-      <c r="F11" s="36" t="n"/>
+      <c r="E11" s="37" t="n"/>
+      <c r="F11" s="37" t="n"/>
     </row>
     <row r="12">
       <c r="D12" s="25" t="n"/>
-      <c r="E12" s="36" t="n"/>
-      <c r="F12" s="36" t="n"/>
+      <c r="E12" s="37" t="n"/>
+      <c r="F12" s="37" t="n"/>
     </row>
     <row r="13">
       <c r="D13" s="25" t="n"/>
-      <c r="E13" s="36" t="n"/>
-      <c r="F13" s="36" t="n"/>
+      <c r="E13" s="37" t="n"/>
+      <c r="F13" s="37" t="n"/>
     </row>
     <row r="14">
       <c r="D14" s="25" t="n"/>
-      <c r="E14" s="36" t="n"/>
-      <c r="F14" s="36" t="n"/>
+      <c r="E14" s="37" t="n"/>
+      <c r="F14" s="37" t="n"/>
     </row>
     <row r="15">
       <c r="D15" s="25" t="n"/>
-      <c r="E15" s="36" t="n"/>
-      <c r="F15" s="36" t="n"/>
+      <c r="E15" s="37" t="n"/>
+      <c r="F15" s="37" t="n"/>
     </row>
     <row r="16">
       <c r="D16" s="25" t="n"/>
-      <c r="E16" s="36" t="n"/>
-      <c r="F16" s="36" t="n"/>
+      <c r="E16" s="37" t="n"/>
+      <c r="F16" s="37" t="n"/>
     </row>
     <row r="17">
       <c r="D17" s="25" t="n"/>
-      <c r="E17" s="36" t="n"/>
-      <c r="F17" s="36" t="n"/>
+      <c r="E17" s="37" t="n"/>
+      <c r="F17" s="37" t="n"/>
     </row>
     <row r="18">
       <c r="D18" s="25" t="n"/>
-      <c r="E18" s="36" t="n"/>
-      <c r="F18" s="36" t="n"/>
+      <c r="E18" s="37" t="n"/>
+      <c r="F18" s="37" t="n"/>
     </row>
     <row r="19">
       <c r="D19" s="25" t="n"/>
-      <c r="E19" s="36" t="n"/>
-      <c r="F19" s="36" t="n"/>
+      <c r="E19" s="37" t="n"/>
+      <c r="F19" s="37" t="n"/>
     </row>
     <row r="20">
       <c r="D20" s="25" t="n"/>
-      <c r="E20" s="36" t="n"/>
-      <c r="F20" s="36" t="n"/>
+      <c r="E20" s="37" t="n"/>
+      <c r="F20" s="37" t="n"/>
     </row>
     <row r="21">
       <c r="D21" s="25" t="n"/>
-      <c r="E21" s="36" t="n"/>
-      <c r="F21" s="36" t="n"/>
+      <c r="E21" s="37" t="n"/>
+      <c r="F21" s="37" t="n"/>
     </row>
     <row r="22">
       <c r="D22" s="25" t="n"/>
-      <c r="E22" s="36" t="n"/>
-      <c r="F22" s="36" t="n"/>
+      <c r="E22" s="37" t="n"/>
+      <c r="F22" s="37" t="n"/>
     </row>
     <row r="23">
       <c r="D23" s="25" t="n"/>
-      <c r="E23" s="36" t="n"/>
-      <c r="F23" s="36" t="n"/>
+      <c r="E23" s="37" t="n"/>
+      <c r="F23" s="37" t="n"/>
     </row>
     <row r="24">
       <c r="D24" s="25" t="n"/>
-      <c r="E24" s="36" t="n"/>
-      <c r="F24" s="36" t="n"/>
+      <c r="E24" s="37" t="n"/>
+      <c r="F24" s="37" t="n"/>
     </row>
     <row r="25">
       <c r="D25" s="25" t="n"/>
-      <c r="E25" s="36" t="n"/>
-      <c r="F25" s="36" t="n"/>
+      <c r="E25" s="37" t="n"/>
+      <c r="F25" s="37" t="n"/>
     </row>
     <row r="26">
       <c r="D26" s="25" t="n"/>
-      <c r="E26" s="36" t="n"/>
-      <c r="F26" s="36" t="n"/>
+      <c r="E26" s="37" t="n"/>
+      <c r="F26" s="37" t="n"/>
     </row>
     <row r="27">
       <c r="D27" s="25" t="n"/>
-      <c r="E27" s="36" t="n"/>
-      <c r="F27" s="36" t="n"/>
+      <c r="E27" s="37" t="n"/>
+      <c r="F27" s="37" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -5291,10 +6238,10 @@
       <c r="D2" s="25" t="n">
         <v>458759412</v>
       </c>
-      <c r="E2" s="36" t="n">
+      <c r="E2" s="37" t="n">
         <v>12942</v>
       </c>
-      <c r="F2" s="36" t="n">
+      <c r="F2" s="37" t="n">
         <v>43927</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -5315,128 +6262,128 @@
     </row>
     <row r="3">
       <c r="D3" s="25" t="n"/>
-      <c r="E3" s="36" t="n"/>
-      <c r="F3" s="36" t="n"/>
+      <c r="E3" s="37" t="n"/>
+      <c r="F3" s="37" t="n"/>
     </row>
     <row r="4">
       <c r="D4" s="25" t="n"/>
-      <c r="E4" s="36" t="n"/>
-      <c r="F4" s="36" t="n"/>
+      <c r="E4" s="37" t="n"/>
+      <c r="F4" s="37" t="n"/>
     </row>
     <row r="5">
       <c r="D5" s="25" t="n"/>
-      <c r="E5" s="36" t="n"/>
-      <c r="F5" s="36" t="n"/>
+      <c r="E5" s="37" t="n"/>
+      <c r="F5" s="37" t="n"/>
     </row>
     <row r="6">
       <c r="D6" s="25" t="n"/>
-      <c r="E6" s="36" t="n"/>
-      <c r="F6" s="36" t="n"/>
+      <c r="E6" s="37" t="n"/>
+      <c r="F6" s="37" t="n"/>
     </row>
     <row r="7">
       <c r="D7" s="25" t="n"/>
-      <c r="E7" s="36" t="n"/>
-      <c r="F7" s="36" t="n"/>
+      <c r="E7" s="37" t="n"/>
+      <c r="F7" s="37" t="n"/>
     </row>
     <row r="8">
       <c r="D8" s="25" t="n"/>
-      <c r="E8" s="36" t="n"/>
-      <c r="F8" s="36" t="n"/>
+      <c r="E8" s="37" t="n"/>
+      <c r="F8" s="37" t="n"/>
     </row>
     <row r="9">
       <c r="D9" s="25" t="n"/>
-      <c r="E9" s="36" t="n"/>
-      <c r="F9" s="36" t="n"/>
+      <c r="E9" s="37" t="n"/>
+      <c r="F9" s="37" t="n"/>
     </row>
     <row r="10">
       <c r="D10" s="25" t="n"/>
-      <c r="E10" s="36" t="n"/>
-      <c r="F10" s="36" t="n"/>
+      <c r="E10" s="37" t="n"/>
+      <c r="F10" s="37" t="n"/>
     </row>
     <row r="11">
       <c r="D11" s="25" t="n"/>
-      <c r="E11" s="36" t="n"/>
-      <c r="F11" s="36" t="n"/>
+      <c r="E11" s="37" t="n"/>
+      <c r="F11" s="37" t="n"/>
     </row>
     <row r="12">
       <c r="D12" s="25" t="n"/>
-      <c r="E12" s="36" t="n"/>
-      <c r="F12" s="36" t="n"/>
+      <c r="E12" s="37" t="n"/>
+      <c r="F12" s="37" t="n"/>
     </row>
     <row r="13">
       <c r="D13" s="25" t="n"/>
-      <c r="E13" s="36" t="n"/>
-      <c r="F13" s="36" t="n"/>
+      <c r="E13" s="37" t="n"/>
+      <c r="F13" s="37" t="n"/>
     </row>
     <row r="14">
       <c r="D14" s="25" t="n"/>
-      <c r="E14" s="36" t="n"/>
-      <c r="F14" s="36" t="n"/>
+      <c r="E14" s="37" t="n"/>
+      <c r="F14" s="37" t="n"/>
     </row>
     <row r="15">
       <c r="D15" s="25" t="n"/>
-      <c r="E15" s="36" t="n"/>
-      <c r="F15" s="36" t="n"/>
+      <c r="E15" s="37" t="n"/>
+      <c r="F15" s="37" t="n"/>
     </row>
     <row r="16">
       <c r="D16" s="25" t="n"/>
-      <c r="E16" s="36" t="n"/>
-      <c r="F16" s="36" t="n"/>
+      <c r="E16" s="37" t="n"/>
+      <c r="F16" s="37" t="n"/>
     </row>
     <row r="17">
       <c r="D17" s="25" t="n"/>
-      <c r="E17" s="36" t="n"/>
-      <c r="F17" s="36" t="n"/>
+      <c r="E17" s="37" t="n"/>
+      <c r="F17" s="37" t="n"/>
     </row>
     <row r="18">
       <c r="D18" s="25" t="n"/>
-      <c r="E18" s="36" t="n"/>
-      <c r="F18" s="36" t="n"/>
+      <c r="E18" s="37" t="n"/>
+      <c r="F18" s="37" t="n"/>
     </row>
     <row r="19">
       <c r="D19" s="25" t="n"/>
-      <c r="E19" s="36" t="n"/>
-      <c r="F19" s="36" t="n"/>
+      <c r="E19" s="37" t="n"/>
+      <c r="F19" s="37" t="n"/>
     </row>
     <row r="20">
       <c r="D20" s="25" t="n"/>
-      <c r="E20" s="36" t="n"/>
-      <c r="F20" s="36" t="n"/>
+      <c r="E20" s="37" t="n"/>
+      <c r="F20" s="37" t="n"/>
     </row>
     <row r="21">
       <c r="D21" s="25" t="n"/>
-      <c r="E21" s="36" t="n"/>
-      <c r="F21" s="36" t="n"/>
+      <c r="E21" s="37" t="n"/>
+      <c r="F21" s="37" t="n"/>
     </row>
     <row r="22">
       <c r="D22" s="25" t="n"/>
-      <c r="E22" s="36" t="n"/>
-      <c r="F22" s="36" t="n"/>
+      <c r="E22" s="37" t="n"/>
+      <c r="F22" s="37" t="n"/>
     </row>
     <row r="23">
       <c r="D23" s="25" t="n"/>
-      <c r="E23" s="36" t="n"/>
-      <c r="F23" s="36" t="n"/>
+      <c r="E23" s="37" t="n"/>
+      <c r="F23" s="37" t="n"/>
     </row>
     <row r="24">
       <c r="D24" s="25" t="n"/>
-      <c r="E24" s="36" t="n"/>
-      <c r="F24" s="36" t="n"/>
+      <c r="E24" s="37" t="n"/>
+      <c r="F24" s="37" t="n"/>
     </row>
     <row r="25">
       <c r="D25" s="25" t="n"/>
-      <c r="E25" s="36" t="n"/>
-      <c r="F25" s="36" t="n"/>
+      <c r="E25" s="37" t="n"/>
+      <c r="F25" s="37" t="n"/>
     </row>
     <row r="26">
       <c r="D26" s="25" t="n"/>
-      <c r="E26" s="36" t="n"/>
-      <c r="F26" s="36" t="n"/>
+      <c r="E26" s="37" t="n"/>
+      <c r="F26" s="37" t="n"/>
     </row>
     <row r="27">
       <c r="D27" s="25" t="n"/>
-      <c r="E27" s="36" t="n"/>
-      <c r="F27" s="36" t="n"/>
+      <c r="E27" s="37" t="n"/>
+      <c r="F27" s="37" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -5528,10 +6475,10 @@
       <c r="D2" s="25" t="n">
         <v>2532525</v>
       </c>
-      <c r="E2" s="36" t="n">
+      <c r="E2" s="37" t="n">
         <v>9379</v>
       </c>
-      <c r="F2" s="36" t="n">
+      <c r="F2" s="37" t="n">
         <v>44141</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -5569,10 +6516,10 @@
       <c r="D3" s="25" t="n">
         <v>453789123</v>
       </c>
-      <c r="E3" s="36" t="n">
+      <c r="E3" s="37" t="n">
         <v>7619</v>
       </c>
-      <c r="F3" s="36" t="n">
+      <c r="F3" s="37" t="n">
         <v>44111</v>
       </c>
       <c r="G3" t="inlineStr">
@@ -5593,123 +6540,123 @@
     </row>
     <row r="4">
       <c r="D4" s="25" t="n"/>
-      <c r="E4" s="36" t="n"/>
-      <c r="F4" s="36" t="n"/>
+      <c r="E4" s="37" t="n"/>
+      <c r="F4" s="37" t="n"/>
     </row>
     <row r="5">
       <c r="D5" s="25" t="n"/>
-      <c r="E5" s="36" t="n"/>
-      <c r="F5" s="36" t="n"/>
+      <c r="E5" s="37" t="n"/>
+      <c r="F5" s="37" t="n"/>
     </row>
     <row r="6">
       <c r="D6" s="25" t="n"/>
-      <c r="E6" s="36" t="n"/>
-      <c r="F6" s="36" t="n"/>
+      <c r="E6" s="37" t="n"/>
+      <c r="F6" s="37" t="n"/>
     </row>
     <row r="7">
       <c r="D7" s="25" t="n"/>
-      <c r="E7" s="36" t="n"/>
-      <c r="F7" s="36" t="n"/>
+      <c r="E7" s="37" t="n"/>
+      <c r="F7" s="37" t="n"/>
     </row>
     <row r="8">
       <c r="D8" s="25" t="n"/>
-      <c r="E8" s="36" t="n"/>
-      <c r="F8" s="36" t="n"/>
+      <c r="E8" s="37" t="n"/>
+      <c r="F8" s="37" t="n"/>
     </row>
     <row r="9">
       <c r="D9" s="25" t="n"/>
-      <c r="E9" s="36" t="n"/>
-      <c r="F9" s="36" t="n"/>
+      <c r="E9" s="37" t="n"/>
+      <c r="F9" s="37" t="n"/>
     </row>
     <row r="10">
       <c r="D10" s="25" t="n"/>
-      <c r="E10" s="36" t="n"/>
-      <c r="F10" s="36" t="n"/>
+      <c r="E10" s="37" t="n"/>
+      <c r="F10" s="37" t="n"/>
     </row>
     <row r="11">
       <c r="D11" s="25" t="n"/>
-      <c r="E11" s="36" t="n"/>
-      <c r="F11" s="36" t="n"/>
+      <c r="E11" s="37" t="n"/>
+      <c r="F11" s="37" t="n"/>
     </row>
     <row r="12">
       <c r="D12" s="25" t="n"/>
-      <c r="E12" s="36" t="n"/>
-      <c r="F12" s="36" t="n"/>
+      <c r="E12" s="37" t="n"/>
+      <c r="F12" s="37" t="n"/>
     </row>
     <row r="13">
       <c r="D13" s="25" t="n"/>
-      <c r="E13" s="36" t="n"/>
-      <c r="F13" s="36" t="n"/>
+      <c r="E13" s="37" t="n"/>
+      <c r="F13" s="37" t="n"/>
     </row>
     <row r="14">
       <c r="D14" s="25" t="n"/>
-      <c r="E14" s="36" t="n"/>
-      <c r="F14" s="36" t="n"/>
+      <c r="E14" s="37" t="n"/>
+      <c r="F14" s="37" t="n"/>
     </row>
     <row r="15">
       <c r="D15" s="25" t="n"/>
-      <c r="E15" s="36" t="n"/>
-      <c r="F15" s="36" t="n"/>
+      <c r="E15" s="37" t="n"/>
+      <c r="F15" s="37" t="n"/>
     </row>
     <row r="16">
       <c r="D16" s="25" t="n"/>
-      <c r="E16" s="36" t="n"/>
-      <c r="F16" s="36" t="n"/>
+      <c r="E16" s="37" t="n"/>
+      <c r="F16" s="37" t="n"/>
     </row>
     <row r="17">
       <c r="D17" s="25" t="n"/>
-      <c r="E17" s="36" t="n"/>
-      <c r="F17" s="36" t="n"/>
+      <c r="E17" s="37" t="n"/>
+      <c r="F17" s="37" t="n"/>
     </row>
     <row r="18">
       <c r="D18" s="25" t="n"/>
-      <c r="E18" s="36" t="n"/>
-      <c r="F18" s="36" t="n"/>
+      <c r="E18" s="37" t="n"/>
+      <c r="F18" s="37" t="n"/>
     </row>
     <row r="19">
       <c r="D19" s="25" t="n"/>
-      <c r="E19" s="36" t="n"/>
-      <c r="F19" s="36" t="n"/>
+      <c r="E19" s="37" t="n"/>
+      <c r="F19" s="37" t="n"/>
     </row>
     <row r="20">
       <c r="D20" s="25" t="n"/>
-      <c r="E20" s="36" t="n"/>
-      <c r="F20" s="36" t="n"/>
+      <c r="E20" s="37" t="n"/>
+      <c r="F20" s="37" t="n"/>
     </row>
     <row r="21">
       <c r="D21" s="25" t="n"/>
-      <c r="E21" s="36" t="n"/>
-      <c r="F21" s="36" t="n"/>
+      <c r="E21" s="37" t="n"/>
+      <c r="F21" s="37" t="n"/>
     </row>
     <row r="22">
       <c r="D22" s="25" t="n"/>
-      <c r="E22" s="36" t="n"/>
-      <c r="F22" s="36" t="n"/>
+      <c r="E22" s="37" t="n"/>
+      <c r="F22" s="37" t="n"/>
     </row>
     <row r="23">
       <c r="D23" s="25" t="n"/>
-      <c r="E23" s="36" t="n"/>
-      <c r="F23" s="36" t="n"/>
+      <c r="E23" s="37" t="n"/>
+      <c r="F23" s="37" t="n"/>
     </row>
     <row r="24">
       <c r="D24" s="25" t="n"/>
-      <c r="E24" s="36" t="n"/>
-      <c r="F24" s="36" t="n"/>
+      <c r="E24" s="37" t="n"/>
+      <c r="F24" s="37" t="n"/>
     </row>
     <row r="25">
       <c r="D25" s="25" t="n"/>
-      <c r="E25" s="36" t="n"/>
-      <c r="F25" s="36" t="n"/>
+      <c r="E25" s="37" t="n"/>
+      <c r="F25" s="37" t="n"/>
     </row>
     <row r="26">
       <c r="D26" s="25" t="n"/>
-      <c r="E26" s="36" t="n"/>
-      <c r="F26" s="36" t="n"/>
+      <c r="E26" s="37" t="n"/>
+      <c r="F26" s="37" t="n"/>
     </row>
     <row r="27">
       <c r="D27" s="25" t="n"/>
-      <c r="E27" s="36" t="n"/>
-      <c r="F27" s="36" t="n"/>
+      <c r="E27" s="37" t="n"/>
+      <c r="F27" s="37" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>